<commit_message>
Adapted AI model, corrected error
</commit_message>
<xml_diff>
--- a/python/api/SEM/BEP/data/carbon.xlsx
+++ b/python/api/SEM/BEP/data/carbon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents Personnels\jlanderc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlanderc\PycharmProjects\cookbook\python\api\SEM\BEP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2510B17-71AB-4EFF-B118-8BBC7AFA0BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A69E56-223F-440F-A53A-EC0354972D89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E50CBFDC-996C-4008-978C-0DEF3980B0F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Diesel</t>
   </si>
@@ -129,22 +129,19 @@
     <t>plane/first</t>
   </si>
   <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>plane</t>
+  </si>
+  <si>
+    <t>carbon_coef</t>
+  </si>
+  <si>
     <t>travel_code</t>
   </si>
   <si>
-    <t>travel_code_id</t>
-  </si>
-  <si>
-    <t>car</t>
-  </si>
-  <si>
-    <t>plane</t>
-  </si>
-  <si>
-    <t>crookness_coef</t>
-  </si>
-  <si>
-    <t>carbon_coef</t>
+    <t>tortuosity_coef</t>
   </si>
 </sst>
 </file>
@@ -760,67 +757,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B15048D-9446-41DA-BE63-7E70F03C418C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>1.24</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>1.24</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2">
         <v>0.11639099999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>1.1499999999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="2">
         <v>3.1075999999999999E-2</v>
       </c>
     </row>

</xml_diff>